<commit_message>
- corrected lots of ugly bugs on pitch and roll - new test buttons for left and right motors separately - new checkbox for disabling pitch and roll
</commit_message>
<xml_diff>
--- a/Simulador Automovel/Damp Lag Compensation.xlsx
+++ b/Simulador Automovel/Damp Lag Compensation.xlsx
@@ -5789,118 +5789,118 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.999999999999996</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.999999999999993</c:v>
+                  <c:v>43.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.8</c:v>
+                  <c:v>57.8125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59.039999999999992</c:v>
+                  <c:v>68.359375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>67.231999999999999</c:v>
+                  <c:v>76.26953125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.785600000000002</c:v>
+                  <c:v>82.2021484375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.028480000000002</c:v>
+                  <c:v>86.651611328125</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>83.222784000000004</c:v>
+                  <c:v>89.98870849609375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86.578227200000001</c:v>
+                  <c:v>92.491531372070313</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>89.262581760000003</c:v>
+                  <c:v>94.368648529052734</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71.410065408000008</c:v>
+                  <c:v>70.776486396789551</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>57.12805232640001</c:v>
+                  <c:v>53.082364797592163</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45.702441861120008</c:v>
+                  <c:v>39.811773598194122</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.561953488896009</c:v>
+                  <c:v>29.858830198645592</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.249562791116809</c:v>
+                  <c:v>22.394122648984194</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.39965023289345</c:v>
+                  <c:v>16.795591986738145</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.71972018631476</c:v>
+                  <c:v>12.596693990053609</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.975776149051809</c:v>
+                  <c:v>9.4475204925402068</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.980620919241447</c:v>
+                  <c:v>7.0856403694051551</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.5844967353931576</c:v>
+                  <c:v>5.3142302770538663</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.6675973883145261</c:v>
+                  <c:v>3.9856727077903997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.1340779106516212</c:v>
+                  <c:v>2.9892545308427998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.9072623285212975</c:v>
+                  <c:v>2.2419408981320998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.9258098628170384</c:v>
+                  <c:v>1.6814556735990749</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.1406478902536308</c:v>
+                  <c:v>1.2610917551993062</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5125183122029049</c:v>
+                  <c:v>0.94581881639947962</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.0100146497623239</c:v>
+                  <c:v>0.70936411229960972</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.6080117198098591</c:v>
+                  <c:v>0.53202308422470734</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2864093758478874</c:v>
+                  <c:v>0.39901731316853051</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.02912750067831</c:v>
+                  <c:v>0.29926298487639791</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.82330200054264813</c:v>
+                  <c:v>0.22444723865729843</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.65864160043411857</c:v>
+                  <c:v>0.16833542899297382</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5269132803472949</c:v>
+                  <c:v>0.12625157174473037</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.42153062427783594</c:v>
+                  <c:v>9.4688678808547783E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.33722449942226879</c:v>
+                  <c:v>7.101650910641083E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.26977959953781505</c:v>
+                  <c:v>5.3262381829808123E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.21582367963025206</c:v>
+                  <c:v>3.9946786372356088E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.17265894370420165</c:v>
+                  <c:v>2.9960089779267066E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15027,7 +15027,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15046,7 +15046,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="20">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>19</v>
@@ -15054,7 +15054,7 @@
       <c r="G1" s="24"/>
       <c r="H1" s="25">
         <f>D1*100/10*(1/B1)</f>
-        <v>0.22857142857142856</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>13</v>
@@ -15112,7 +15112,7 @@
       </c>
       <c r="D4" s="19">
         <f>D3*D$1+C4*(1-D$1)</f>
-        <v>19.999999999999996</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -15128,7 +15128,7 @@
       </c>
       <c r="D5" s="19">
         <f t="shared" ref="D5:D41" si="1">D4*D$1+C5*(1-D$1)</f>
-        <v>35.999999999999993</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -15144,7 +15144,7 @@
       </c>
       <c r="D6" s="19">
         <f t="shared" si="1"/>
-        <v>48.8</v>
+        <v>57.8125</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -15160,7 +15160,7 @@
       </c>
       <c r="D7" s="19">
         <f t="shared" si="1"/>
-        <v>59.039999999999992</v>
+        <v>68.359375</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -15176,7 +15176,7 @@
       </c>
       <c r="D8" s="19">
         <f t="shared" si="1"/>
-        <v>67.231999999999999</v>
+        <v>76.26953125</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -15192,7 +15192,7 @@
       </c>
       <c r="D9" s="19">
         <f t="shared" si="1"/>
-        <v>73.785600000000002</v>
+        <v>82.2021484375</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -15208,7 +15208,7 @@
       </c>
       <c r="D10" s="19">
         <f t="shared" si="1"/>
-        <v>79.028480000000002</v>
+        <v>86.651611328125</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -15224,7 +15224,7 @@
       </c>
       <c r="D11" s="19">
         <f t="shared" si="1"/>
-        <v>83.222784000000004</v>
+        <v>89.98870849609375</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -15240,7 +15240,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" si="1"/>
-        <v>86.578227200000001</v>
+        <v>92.491531372070313</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -15256,7 +15256,7 @@
       </c>
       <c r="D13" s="19">
         <f t="shared" si="1"/>
-        <v>89.262581760000003</v>
+        <v>94.368648529052734</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -15272,7 +15272,7 @@
       </c>
       <c r="D14" s="19">
         <f t="shared" si="1"/>
-        <v>71.410065408000008</v>
+        <v>70.776486396789551</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -15288,7 +15288,7 @@
       </c>
       <c r="D15" s="19">
         <f t="shared" si="1"/>
-        <v>57.12805232640001</v>
+        <v>53.082364797592163</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -15304,7 +15304,7 @@
       </c>
       <c r="D16" s="19">
         <f t="shared" si="1"/>
-        <v>45.702441861120008</v>
+        <v>39.811773598194122</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -15320,7 +15320,7 @@
       </c>
       <c r="D17" s="19">
         <f t="shared" si="1"/>
-        <v>36.561953488896009</v>
+        <v>29.858830198645592</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -15336,7 +15336,7 @@
       </c>
       <c r="D18" s="19">
         <f t="shared" si="1"/>
-        <v>29.249562791116809</v>
+        <v>22.394122648984194</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -15352,7 +15352,7 @@
       </c>
       <c r="D19" s="19">
         <f t="shared" si="1"/>
-        <v>23.39965023289345</v>
+        <v>16.795591986738145</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -15368,7 +15368,7 @@
       </c>
       <c r="D20" s="19">
         <f t="shared" si="1"/>
-        <v>18.71972018631476</v>
+        <v>12.596693990053609</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -15384,7 +15384,7 @@
       </c>
       <c r="D21" s="19">
         <f t="shared" si="1"/>
-        <v>14.975776149051809</v>
+        <v>9.4475204925402068</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -15400,7 +15400,7 @@
       </c>
       <c r="D22" s="19">
         <f t="shared" si="1"/>
-        <v>11.980620919241447</v>
+        <v>7.0856403694051551</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -15416,7 +15416,7 @@
       </c>
       <c r="D23" s="19">
         <f t="shared" si="1"/>
-        <v>9.5844967353931576</v>
+        <v>5.3142302770538663</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -15432,7 +15432,7 @@
       </c>
       <c r="D24" s="19">
         <f t="shared" si="1"/>
-        <v>7.6675973883145261</v>
+        <v>3.9856727077903997</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -15448,7 +15448,7 @@
       </c>
       <c r="D25" s="19">
         <f t="shared" si="1"/>
-        <v>6.1340779106516212</v>
+        <v>2.9892545308427998</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -15464,7 +15464,7 @@
       </c>
       <c r="D26" s="19">
         <f t="shared" si="1"/>
-        <v>4.9072623285212975</v>
+        <v>2.2419408981320998</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -15480,7 +15480,7 @@
       </c>
       <c r="D27" s="19">
         <f t="shared" si="1"/>
-        <v>3.9258098628170384</v>
+        <v>1.6814556735990749</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -15496,7 +15496,7 @@
       </c>
       <c r="D28" s="19">
         <f t="shared" si="1"/>
-        <v>3.1406478902536308</v>
+        <v>1.2610917551993062</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -15512,7 +15512,7 @@
       </c>
       <c r="D29" s="19">
         <f t="shared" si="1"/>
-        <v>2.5125183122029049</v>
+        <v>0.94581881639947962</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -15528,7 +15528,7 @@
       </c>
       <c r="D30" s="19">
         <f t="shared" si="1"/>
-        <v>2.0100146497623239</v>
+        <v>0.70936411229960972</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -15544,7 +15544,7 @@
       </c>
       <c r="D31" s="19">
         <f t="shared" si="1"/>
-        <v>1.6080117198098591</v>
+        <v>0.53202308422470734</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -15560,7 +15560,7 @@
       </c>
       <c r="D32" s="19">
         <f t="shared" si="1"/>
-        <v>1.2864093758478874</v>
+        <v>0.39901731316853051</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -15576,7 +15576,7 @@
       </c>
       <c r="D33" s="19">
         <f t="shared" si="1"/>
-        <v>1.02912750067831</v>
+        <v>0.29926298487639791</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -15592,7 +15592,7 @@
       </c>
       <c r="D34" s="19">
         <f t="shared" si="1"/>
-        <v>0.82330200054264813</v>
+        <v>0.22444723865729843</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -15608,7 +15608,7 @@
       </c>
       <c r="D35" s="19">
         <f t="shared" si="1"/>
-        <v>0.65864160043411857</v>
+        <v>0.16833542899297382</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -15624,7 +15624,7 @@
       </c>
       <c r="D36" s="19">
         <f t="shared" si="1"/>
-        <v>0.5269132803472949</v>
+        <v>0.12625157174473037</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -15640,7 +15640,7 @@
       </c>
       <c r="D37" s="19">
         <f t="shared" si="1"/>
-        <v>0.42153062427783594</v>
+        <v>9.4688678808547783E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -15656,7 +15656,7 @@
       </c>
       <c r="D38" s="19">
         <f t="shared" si="1"/>
-        <v>0.33722449942226879</v>
+        <v>7.101650910641083E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -15672,7 +15672,7 @@
       </c>
       <c r="D39" s="19">
         <f t="shared" si="1"/>
-        <v>0.26977959953781505</v>
+        <v>5.3262381829808123E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -15688,7 +15688,7 @@
       </c>
       <c r="D40" s="19">
         <f t="shared" si="1"/>
-        <v>0.21582367963025206</v>
+        <v>3.9946786372356088E-2</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -15704,7 +15704,7 @@
       </c>
       <c r="D41" s="19">
         <f t="shared" si="1"/>
-        <v>0.17265894370420165</v>
+        <v>2.9960089779267066E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chkArduinoTime. chkDisableFF. Simple ErrorLog.
</commit_message>
<xml_diff>
--- a/Simulador Automovel/Damp Lag Compensation.xlsx
+++ b/Simulador Automovel/Damp Lag Compensation.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15270" windowHeight="7665" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15270" windowHeight="7665" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Exponential ratios" sheetId="1" r:id="rId1"/>
     <sheet name="Damp Lag Compensation" sheetId="2" r:id="rId2"/>
     <sheet name="Temperature OverHeat" sheetId="3" r:id="rId3"/>
     <sheet name="Inertia" sheetId="4" r:id="rId4"/>
+    <sheet name="Folha1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>normal</t>
   </si>
@@ -81,6 +82,15 @@
   <si>
     <t>Time to reach 6%:</t>
   </si>
+  <si>
+    <t>Km/H</t>
+  </si>
+  <si>
+    <t>M/s</t>
+  </si>
+  <si>
+    <t>Rot/s</t>
+  </si>
 </sst>
 </file>
 
@@ -89,8 +99,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -190,8 +200,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -217,20 +227,7 @@
     <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -245,10 +242,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.9113298337707819E-2"/>
+          <c:x val="7.9113298337707832E-2"/>
           <c:y val="2.8252405949256338E-2"/>
-          <c:w val="0.65426159230096259"/>
-          <c:h val="0.83062919218431075"/>
+          <c:w val="0.6542615923009627"/>
+          <c:h val="0.83062919218431086"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -710,25 +707,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112853376"/>
-        <c:axId val="112883200"/>
+        <c:axId val="71032832"/>
+        <c:axId val="71034368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112853376"/>
+        <c:axId val="71032832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112883200"/>
+        <c:crossAx val="71034368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112883200"/>
+        <c:axId val="71034368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +733,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112853376"/>
+        <c:crossAx val="71032832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -749,7 +746,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -766,8 +763,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.7801651180778733E-2"/>
-          <c:y val="1.3932693344838746E-2"/>
-          <c:w val="0.85671000126217278"/>
+          <c:y val="1.3932693344838749E-2"/>
+          <c:w val="0.85671000126217289"/>
           <c:h val="0.9517805876871257"/>
         </c:manualLayout>
       </c:layout>
@@ -897,8 +894,8 @@
         </c:ser>
         <c:gapWidth val="18"/>
         <c:overlap val="-1"/>
-        <c:axId val="109432192"/>
-        <c:axId val="114521216"/>
+        <c:axId val="75669504"/>
+        <c:axId val="75671040"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1508,24 +1505,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109432192"/>
-        <c:axId val="114521216"/>
+        <c:axId val="75669504"/>
+        <c:axId val="75671040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109432192"/>
+        <c:axId val="75669504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114521216"/>
+        <c:crossAx val="75671040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114521216"/>
+        <c:axId val="75671040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,7 +1530,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109432192"/>
+        <c:crossAx val="75669504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1547,7 +1544,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1564,7 +1561,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.9802434767596498E-2"/>
-          <c:y val="2.8252405949256341E-2"/>
+          <c:y val="2.8252405949256338E-2"/>
           <c:w val="0.94939244105278209"/>
           <c:h val="0.91108778069407992"/>
         </c:manualLayout>
@@ -3489,8 +3486,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49859200"/>
-        <c:axId val="50065792"/>
+        <c:axId val="75766016"/>
+        <c:axId val="75776000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5415,25 +5412,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="49859200"/>
-        <c:axId val="50065792"/>
+        <c:axId val="75766016"/>
+        <c:axId val="75776000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49859200"/>
+        <c:axId val="75766016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50065792"/>
+        <c:crossAx val="75776000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50065792"/>
+        <c:axId val="75776000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5441,7 +5438,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49859200"/>
+        <c:crossAx val="75766016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5452,10 +5449,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88504962059598669"/>
-          <c:y val="8.8754009915427267E-3"/>
-          <c:w val="0.10863686815267494"/>
-          <c:h val="0.10303654350898446"/>
+          <c:x val="0.8850496205959868"/>
+          <c:y val="8.8754009915427302E-3"/>
+          <c:w val="0.10863686815267495"/>
+          <c:h val="0.10303654350898449"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -5464,7 +5461,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5480,9 +5477,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.3851718928061299E-2"/>
+          <c:x val="4.3851718928061306E-2"/>
           <c:y val="2.9966314939377518E-2"/>
-          <c:w val="0.90269706954607098"/>
+          <c:w val="0.9026970695460711"/>
           <c:h val="0.90241788602335637"/>
         </c:manualLayout>
       </c:layout>
@@ -5631,8 +5628,8 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="11"/>
-        <c:axId val="130639360"/>
-        <c:axId val="191996672"/>
+        <c:axId val="75818496"/>
+        <c:axId val="75820032"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5907,11 +5904,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="130639360"/>
-        <c:axId val="191996672"/>
+        <c:axId val="75818496"/>
+        <c:axId val="75820032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="130639360"/>
+        <c:axId val="75818496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5929,14 +5926,14 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191996672"/>
+        <c:crossAx val="75820032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="400"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191996672"/>
+        <c:axId val="75820032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5944,7 +5941,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130639360"/>
+        <c:crossAx val="75818496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5958,7 +5955,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -15026,7 +15023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -15711,4 +15708,126 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4">
+        <f>A2/3.6</f>
+        <v>13.888888888888889</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2/2</f>
+        <v>6.9444444444444446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4">
+        <f t="shared" ref="B3:B8" si="0">A3/3.6</f>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C8" si="1">B3/2</f>
+        <v>13.888888888888889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>150</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" si="0"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="1"/>
+        <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>200</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="0"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="1"/>
+        <v>27.777777777777779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>250</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="0"/>
+        <v>69.444444444444443</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>34.722222222222221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="0"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>350</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>97.222222222222214</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="1"/>
+        <v>48.611111111111107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>